<commit_message>
BUG Report with attachement
</commit_message>
<xml_diff>
--- a/BoschClaims.xlsx
+++ b/BoschClaims.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="124">
   <si>
     <t>Updated By:-</t>
   </si>
@@ -382,9 +382,6 @@
     <t xml:space="preserve">Fail </t>
   </si>
   <si>
-    <t>TimeZoneIssue</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -765,6 +762,141 @@
       </rPr>
       <t>fields blank.             2)Enter valid details in the remianing fields.             3)Click On Save Button.</t>
     </r>
+  </si>
+  <si>
+    <t>1)URL-http://13.126.69.89/bosch/index.php
+2)User name-bhavya-123
+and pwd-Welcome@1234567</t>
+  </si>
+  <si>
+    <t>1)Enter valid URL
+2)Login with valid user name pwd
+3)Click on SP-Claims module 
+4)Click on +Add Claim</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>User should get navigate to the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> Creating New BOSCH - Claims </t>
+    </r>
+  </si>
+  <si>
+    <t>To verify the Creating New BOSCH-Claims page</t>
+  </si>
+  <si>
+    <t>User is on Creating New BOSCH-Claims page</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">There is minor alignment for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Previous Visit Date </t>
+    </r>
+  </si>
+  <si>
+    <t>all the mandatory fileds and alignment should be proper</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Service Package number 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BSP207111</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Job Card-FDGRTGI8RET</t>
+  </si>
+  <si>
+    <t>User should not be able to create  New BOSCH - Claims  and the system must display a proper and specific validation message for  REC Sales Number field " This field is required."                                                              Note: On the basis of REC sales number rest of the  Claims Details should get appear and they should be non editable</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of Job Card 
+06-11-2020
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dealer should be able to create New BOSCH-Claims and there should be validation for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Date of Job Card</t>
+    </r>
+  </si>
+  <si>
+    <t>Date of job card is accepting more than 15 days from the current date</t>
+  </si>
+  <si>
+    <t>master not updated</t>
+  </si>
+  <si>
+    <t>SP Claims_TC_22</t>
+  </si>
+  <si>
+    <t>SP Claims_TC_23</t>
+  </si>
+  <si>
+    <t>Service Package Plan 
+reflecting incorrect data</t>
+  </si>
+  <si>
+    <t>Current visit fields is missing logic and aslo visiting multiple of time</t>
   </si>
 </sst>
 </file>
@@ -772,10 +904,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="dd\-mm\-yyyy"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -888,8 +1020,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -950,8 +1103,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF95B3D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1026,13 +1191,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1061,98 +1247,130 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 2 2" xfId="2"/>
@@ -1433,10 +1651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,38 +1664,39 @@
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="8" max="8" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
       <c r="I1" s="6"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="12" t="s">
+      <c r="E2" s="35"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="10" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="9" t="s">
@@ -1488,18 +1707,18 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="36">
         <v>44187</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="11"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="33"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
       <c r="I3" s="6"/>
@@ -1507,49 +1726,51 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12" t="s">
+      <c r="F4" s="33"/>
+      <c r="G4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="12"/>
+      <c r="H4" s="10">
+        <v>13445</v>
+      </c>
       <c r="I4" s="6"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="11" t="s">
         <v>16</v>
       </c>
       <c r="I5" s="7" t="s">
@@ -1563,431 +1784,538 @@
       </c>
     </row>
     <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+    <row r="7" spans="1:11" s="43" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="I7" s="49"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="49" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D8" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18" t="s">
+      <c r="E8" s="40"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13" t="s">
         <v>26</v>
-      </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="18" t="s">
-        <v>30</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" ht="165" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="K8" s="45" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="45" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="45" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C11" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D11" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="47" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="5" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="37" t="s">
+      <c r="C14" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="37" t="s">
+      <c r="D14" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="5" customFormat="1" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="5" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="C12" s="37" t="s">
+      <c r="D15" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="5" customFormat="1" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="5" customFormat="1" ht="153" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="C13" s="37" t="s">
+      <c r="D16" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="5" customFormat="1" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="C14" s="37" t="s">
+      <c r="D17" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="37" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" s="37" t="s">
+      <c r="D18" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F18" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21" t="s">
+      <c r="D19" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" s="37" t="s">
+      <c r="K19" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17" s="37" t="s">
+      <c r="D20" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="C18" s="37" t="s">
+      <c r="D21" s="29"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="G21" s="16"/>
+      <c r="H21" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="37" t="s">
+      <c r="D22" s="29"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="37" t="s">
+      <c r="D23" s="29"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="37"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="B21" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="37" t="s">
+      <c r="D24" s="30"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="37"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="37" t="s">
+      <c r="D25" s="30"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="38"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="37" t="s">
+      <c r="D26" s="30"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A27" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="38"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="37" t="s">
+      <c r="D27" s="30"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="38"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="37" t="s">
+      <c r="D28" s="30"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="38"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="38"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="38"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21" t="s">
+      <c r="D29" s="30"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="33" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="34" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="35" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2001,6 +2329,8 @@
     <row r="43" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="44" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="45" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B4:C4"/>
@@ -2021,7 +2351,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2032,65 +2362,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="A1" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="20" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="21">
+        <v>23</v>
+      </c>
+      <c r="C4" s="21">
+        <v>15</v>
+      </c>
+      <c r="D4" s="22">
+        <v>11</v>
+      </c>
+      <c r="E4" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="27">
-        <v>21</v>
-      </c>
-      <c r="C4" s="27">
-        <v>0</v>
-      </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="31">
-        <v>21</v>
-      </c>
-      <c r="C5" s="31">
-        <v>0</v>
-      </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="33"/>
+      <c r="B5" s="25">
+        <v>23</v>
+      </c>
+      <c r="C5" s="25">
+        <v>15</v>
+      </c>
+      <c r="D5" s="26">
+        <v>11</v>
+      </c>
+      <c r="E5" s="27">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>